<commit_message>
Code check-in for Resolved Attendance issue
</commit_message>
<xml_diff>
--- a/AnandERP/AERP.Web.UI/Content/DownloadFiles/EmployeeMasterExcelUpload.xlsx
+++ b/AnandERP/AERP.Web.UI/Content/DownloadFiles/EmployeeMasterExcelUpload.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Employee Details" sheetId="1" r:id="Ra355dee56f104fed"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Employee Details" sheetId="1" r:id="Rc04544df8dd04494"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -164,81 +164,6 @@
   </x:si>
   <x:si>
     <x:t>Relation</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Emp12</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Vinit  Thakre</x:t>
-  </x:si>
-  <x:si>
-    <x:t>AGHO</x:t>
-  </x:si>
-  <x:si>
-    <x:t/>
-  </x:si>
-  <x:si>
-    <x:t>Manager</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Accounts</x:t>
-  </x:si>
-  <x:si>
-    <x:t/>
-  </x:si>
-  <x:si>
-    <x:t/>
-  </x:si>
-  <x:si>
-    <x:t/>
-  </x:si>
-  <x:si>
-    <x:t>01 Jan 2018</x:t>
-  </x:si>
-  <x:si>
-    <x:t/>
-  </x:si>
-  <x:si>
-    <x:t/>
-  </x:si>
-  <x:si>
-    <x:t/>
-  </x:si>
-  <x:si>
-    <x:t/>
-  </x:si>
-  <x:si>
-    <x:t/>
-  </x:si>
-  <x:si>
-    <x:t/>
-  </x:si>
-  <x:si>
-    <x:t/>
-  </x:si>
-  <x:si>
-    <x:t/>
-  </x:si>
-  <x:si>
-    <x:t>Male</x:t>
-  </x:si>
-  <x:si>
-    <x:t/>
-  </x:si>
-  <x:si>
-    <x:t/>
-  </x:si>
-  <x:si>
-    <x:t/>
-  </x:si>
-  <x:si>
-    <x:t/>
-  </x:si>
-  <x:si>
-    <x:t/>
   </x:si>
 </x:sst>
 </file>
@@ -697,86 +622,6 @@
         <x:v>51</x:v>
       </x:c>
     </x:row>
-    <x:row r="3">
-      <x:c r="A3" t="s">
-        <x:v>52</x:v>
-      </x:c>
-      <x:c r="B3" t="s">
-        <x:v>53</x:v>
-      </x:c>
-      <x:c r="C3" t="s">
-        <x:v>54</x:v>
-      </x:c>
-      <x:c r="D3" t="s">
-        <x:v>55</x:v>
-      </x:c>
-      <x:c r="F3" t="s">
-        <x:v>56</x:v>
-      </x:c>
-      <x:c r="G3" t="s">
-        <x:v>57</x:v>
-      </x:c>
-      <x:c r="I3" t="s">
-        <x:v>58</x:v>
-      </x:c>
-      <x:c r="L3" t="s">
-        <x:v>59</x:v>
-      </x:c>
-      <x:c r="M3" t="s">
-        <x:v>60</x:v>
-      </x:c>
-      <x:c r="N3" t="s">
-        <x:v>61</x:v>
-      </x:c>
-      <x:c r="O3" t="s">
-        <x:v>62</x:v>
-      </x:c>
-      <x:c r="P3" t="s">
-        <x:v>63</x:v>
-      </x:c>
-      <x:c r="Q3" t="s">
-        <x:v>64</x:v>
-      </x:c>
-      <x:c r="S3" t="s">
-        <x:v>65</x:v>
-      </x:c>
-      <x:c r="T3" t="s">
-        <x:v>66</x:v>
-      </x:c>
-      <x:c r="U3" t="s">
-        <x:v>67</x:v>
-      </x:c>
-      <x:c r="V3" t="s">
-        <x:v>68</x:v>
-      </x:c>
-      <x:c r="W3" t="s">
-        <x:v>69</x:v>
-      </x:c>
-      <x:c r="X3" t="s">
-        <x:v>70</x:v>
-      </x:c>
-      <x:c r="Y3" t="s">
-        <x:v>71</x:v>
-      </x:c>
-      <x:c r="Z3" t="s">
-        <x:v>72</x:v>
-      </x:c>
-      <x:c r="AA3" t="s">
-        <x:v>73</x:v>
-      </x:c>
-      <x:c r="AB3" t="s">
-        <x:v>74</x:v>
-      </x:c>
-      <x:c r="AC3" t="s">
-        <x:v>75</x:v>
-      </x:c>
-      <x:c r="AD3" t="s">
-        <x:v>56</x:v>
-      </x:c>
-      <x:c r="CA3" t="s">
-        <x:v>76</x:v>
-      </x:c>
-    </x:row>
   </x:sheetData>
   <x:mergeCells>
     <x:mergeCell ref="Z1:AD1"/>

</xml_diff>